<commit_message>
Adicionando feature de skill na gupy
</commit_message>
<xml_diff>
--- a/data/data_raw/vagas_gupy_raw.xlsx
+++ b/data/data_raw/vagas_gupy_raw.xlsx
@@ -5339,7 +5339,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -5403,11 +5403,11 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -5742,7 +5742,7 @@
     <col min="17" max="17" style="6" width="11.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="60">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="62.25">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -5844,7 +5844,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="60">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="62.25">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -5893,7 +5893,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="60.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="63">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="60.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="63">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -5991,7 +5991,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="60.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="63">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="60">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="62.25">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -6089,7 +6089,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="61.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="63.75">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>

</xml_diff>